<commit_message>
Added some science files
</commit_message>
<xml_diff>
--- a/obsidian-notes/spreadsheets/periodic-table.xlsx
+++ b/obsidian-notes/spreadsheets/periodic-table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4179229009c49077/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sharm\iCloudDrive\iCloud~md~obsidian\Ishan's notes\Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="315" documentId="8_{A2DA0BEF-85C8-43DE-972C-1F49E8052D81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47000D94-C847-4A89-9F06-1E83D43F14C3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802349D7-9128-4AD6-9FA7-51369F23005D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" xr2:uid="{267BF456-EDF0-4F7C-AF2E-F688F98756E9}"/>
   </bookViews>
@@ -338,9 +338,6 @@
     <t>Ja</t>
   </si>
   <si>
-    <t>*Janium named after ninth planet, Janus</t>
-  </si>
-  <si>
     <t>Vestium</t>
   </si>
   <si>
@@ -666,6 +663,9 @@
   </si>
   <si>
     <t>*Popularium named by a Brit after "the people"</t>
+  </si>
+  <si>
+    <t>*Janium named after eighth planet, Janus</t>
   </si>
 </sst>
 </file>
@@ -819,10 +819,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1124,8 +1120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1273159-333D-42AD-962D-D978BF869110}">
   <dimension ref="B2:K86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1167,13 +1163,13 @@
         <v>35</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="2:11" s="4" customFormat="1" ht="10.5" x14ac:dyDescent="0.4">
@@ -1190,13 +1186,13 @@
         <v>3</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="2:11" s="4" customFormat="1" ht="10.5" x14ac:dyDescent="0.4">
@@ -1236,7 +1232,7 @@
         <v>54</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="2:11" s="4" customFormat="1" ht="10.5" x14ac:dyDescent="0.4">
@@ -1256,7 +1252,7 @@
         <v>8</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.55000000000000004">
@@ -1295,7 +1291,7 @@
     </row>
     <row r="10" spans="2:11" s="5" customFormat="1" ht="23.1" x14ac:dyDescent="0.85">
       <c r="E10" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>58</v>
@@ -1305,28 +1301,28 @@
       </c>
       <c r="H10" s="1"/>
       <c r="J10" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="11" spans="2:11" s="6" customFormat="1" ht="10.5" x14ac:dyDescent="0.4">
       <c r="E11" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H11" s="3"/>
       <c r="J11" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12" spans="2:11" s="4" customFormat="1" ht="10.5" x14ac:dyDescent="0.4">
@@ -1357,14 +1353,14 @@
         <v>60</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H13" s="1"/>
       <c r="J13" s="1" t="s">
         <v>97</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="14" spans="2:11" s="6" customFormat="1" ht="10.5" x14ac:dyDescent="0.4">
@@ -1375,14 +1371,14 @@
         <v>11</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H14" s="3"/>
       <c r="J14" s="3" t="s">
         <v>96</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="15" spans="2:11" s="4" customFormat="1" ht="10.5" x14ac:dyDescent="0.4">
@@ -1413,14 +1409,14 @@
         <v>95</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H16" s="1"/>
       <c r="J16" s="1" t="s">
         <v>93</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="5:11" s="6" customFormat="1" ht="10.5" x14ac:dyDescent="0.4">
@@ -1431,14 +1427,14 @@
         <v>94</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H17" s="3"/>
       <c r="J17" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="18" spans="5:11" s="4" customFormat="1" ht="10.5" x14ac:dyDescent="0.4">
@@ -1466,14 +1462,14 @@
         <v>41</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H19" s="1"/>
       <c r="J19" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>79</v>
@@ -1484,14 +1480,14 @@
         <v>14</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H20" s="3"/>
       <c r="J20" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K20" s="3" t="s">
         <v>80</v>
@@ -1522,14 +1518,14 @@
         <v>76</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>55</v>
       </c>
       <c r="H22" s="1"/>
       <c r="J22" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>99</v>
@@ -1540,14 +1536,14 @@
         <v>15</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H23" s="3"/>
       <c r="J23" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K23" s="3" t="s">
         <v>98</v>
@@ -1578,14 +1574,14 @@
         <v>62</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H25" s="1"/>
       <c r="J25" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>82</v>
@@ -1596,14 +1592,14 @@
         <v>16</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H26" s="3"/>
       <c r="J26" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K26" s="3" t="s">
         <v>81</v>
@@ -1634,14 +1630,14 @@
         <v>36</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H28" s="1"/>
       <c r="J28" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K28" s="1"/>
     </row>
@@ -1650,14 +1646,14 @@
         <v>17</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H29" s="3"/>
       <c r="J29" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K29" s="3"/>
     </row>
@@ -1686,14 +1682,14 @@
         <v>75</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H31" s="1"/>
       <c r="J31" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K31" s="1"/>
     </row>
@@ -1702,14 +1698,14 @@
         <v>18</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H32" s="3"/>
       <c r="J32" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K32" s="3"/>
     </row>
@@ -1745,7 +1741,7 @@
       </c>
       <c r="H34" s="1"/>
       <c r="J34" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K34" s="1"/>
     </row>
@@ -1761,7 +1757,7 @@
       </c>
       <c r="H35" s="3"/>
       <c r="J35" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K35" s="3"/>
     </row>
@@ -1790,14 +1786,14 @@
         <v>72</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>71</v>
       </c>
       <c r="H37" s="1"/>
       <c r="J37" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K37" s="1"/>
     </row>
@@ -1806,14 +1802,14 @@
         <v>20</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G38" s="3" t="s">
         <v>31</v>
       </c>
       <c r="H38" s="3"/>
       <c r="J38" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K38" s="3"/>
     </row>
@@ -1851,17 +1847,17 @@
         <v>70</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>92</v>
       </c>
       <c r="H40" s="1"/>
       <c r="J40" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K40" s="1"/>
     </row>
@@ -1873,17 +1869,17 @@
         <v>21</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H41" s="3"/>
       <c r="J41" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K41" s="3"/>
     </row>
@@ -1953,7 +1949,7 @@
       </c>
       <c r="H44" s="3"/>
       <c r="J44" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K44" s="3"/>
     </row>
@@ -1997,11 +1993,11 @@
         <v>90</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H46" s="1"/>
       <c r="J46" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K46" s="1"/>
     </row>
@@ -2019,11 +2015,11 @@
         <v>89</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H47" s="3"/>
       <c r="J47" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K47" s="3"/>
     </row>
@@ -2067,11 +2063,11 @@
         <v>88</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H49" s="1"/>
       <c r="J49" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K49" s="1"/>
     </row>
@@ -2089,11 +2085,11 @@
         <v>87</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H50" s="3"/>
       <c r="J50" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K50" s="3"/>
     </row>
@@ -2128,10 +2124,10 @@
         <v>66</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H52" s="1"/>
     </row>
@@ -2146,10 +2142,10 @@
         <v>33</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H53" s="3"/>
     </row>
@@ -2181,13 +2177,13 @@
         <v>77</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>73</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>41</v>
@@ -2202,40 +2198,40 @@
         <v>28</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>74</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H56" s="3"/>
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B59" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="60" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B60" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="61" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B61" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="62" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B62" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="63" spans="2:11" x14ac:dyDescent="0.55000000000000004">
@@ -2245,117 +2241,117 @@
     </row>
     <row r="64" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B64" t="s">
-        <v>100</v>
+        <v>209</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B65" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B66" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B67" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B68" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B69" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B70" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B71" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B72" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B73" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B74" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B75" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B76" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B77" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B78" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B79" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B80" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B81" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B82" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B83" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B84" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B85" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B86" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>